<commit_message>
add labels in the column name mapping sheet
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@82576 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/Gates/ontology mapping of gates terms.xlsx
+++ b/Load/src/ontology/Gates/ontology mapping of gates terms.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19460" tabRatio="553"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="25280" windowHeight="13780" tabRatio="553" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="gate term mapping" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2001" uniqueCount="897">
   <si>
     <t>Term IRI</t>
   </si>
@@ -2611,9 +2611,6 @@
     <t>GATES_0000074</t>
   </si>
   <si>
-    <t>won't used by search, used to relate subject to investigation location information</t>
-  </si>
-  <si>
     <t>string values of column 'sstest'</t>
   </si>
   <si>
@@ -2717,6 +2714,12 @@
   </si>
   <si>
     <t>http://purl.bioontology.org/ontology/MEDDRA/10040785</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>won't used by search, used to relate subject to investigation location information, also it has souce_id but won't be added in the ontology</t>
   </si>
 </sst>
 </file>
@@ -2827,8 +2830,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="655">
+  <cellStyleXfs count="663">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3517,7 +3528,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="655">
+  <cellStyles count="663">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3845,6 +3856,10 @@
     <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4172,6 +4187,10 @@
     <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4503,8 +4522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="I53" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="I129" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I65" sqref="I65"/>
@@ -4544,7 +4563,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I1" t="s">
         <v>506</v>
@@ -6357,7 +6376,7 @@
       </c>
       <c r="H65" s="7"/>
       <c r="I65" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="J65" s="22">
         <v>10005329</v>
@@ -6387,7 +6406,7 @@
       </c>
       <c r="H66" s="7"/>
       <c r="I66" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="J66" s="22">
         <v>10010331</v>
@@ -6417,7 +6436,7 @@
       </c>
       <c r="H67" s="7"/>
       <c r="I67" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="J67" s="22">
         <v>10015919</v>
@@ -6447,7 +6466,7 @@
       </c>
       <c r="H68" s="7"/>
       <c r="I68" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="J68" s="22">
         <v>10017947</v>
@@ -6477,7 +6496,7 @@
       </c>
       <c r="H69" s="7"/>
       <c r="I69" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="J69" s="22">
         <v>10018065</v>
@@ -6507,7 +6526,7 @@
       </c>
       <c r="H70" s="7"/>
       <c r="I70" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="J70" s="22">
         <v>10021428</v>
@@ -6537,7 +6556,7 @@
       </c>
       <c r="H71" s="7"/>
       <c r="I71" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="J71" s="22">
         <v>10021881</v>
@@ -6567,7 +6586,7 @@
       </c>
       <c r="H72" s="7"/>
       <c r="I72" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="J72" s="22">
         <v>10022117</v>
@@ -6597,7 +6616,7 @@
       </c>
       <c r="H73" s="7"/>
       <c r="I73" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="J73" s="22">
         <v>10027433</v>
@@ -6627,7 +6646,7 @@
       </c>
       <c r="H74" s="7"/>
       <c r="I74" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="J74" s="22">
         <v>10028395</v>
@@ -6657,7 +6676,7 @@
       </c>
       <c r="H75" s="7"/>
       <c r="I75" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="J75" s="22">
         <v>10029205</v>
@@ -6687,7 +6706,7 @@
       </c>
       <c r="H76" s="7"/>
       <c r="I76" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="J76" s="22">
         <v>10038359</v>
@@ -6717,7 +6736,7 @@
       </c>
       <c r="H77" s="7"/>
       <c r="I77" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="J77" s="22">
         <v>10038738</v>
@@ -6747,7 +6766,7 @@
       </c>
       <c r="H78" s="7"/>
       <c r="I78" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="J78" s="22">
         <v>10040785</v>
@@ -9028,13 +9047,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G158"/>
+  <dimension ref="A1:H158"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9042,11 +9061,12 @@
     <col min="2" max="2" width="39.33203125" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="48" customWidth="1"/>
+    <col min="5" max="5" width="34.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="9" t="s">
         <v>744</v>
       </c>
@@ -9060,13 +9080,16 @@
         <v>768</v>
       </c>
       <c r="E1" t="s">
+        <v>895</v>
+      </c>
+      <c r="F1" t="s">
         <v>704</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="10" t="s">
         <v>189</v>
       </c>
@@ -9080,10 +9103,13 @@
         <v>78</v>
       </c>
       <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="10" t="s">
         <v>189</v>
       </c>
@@ -9097,10 +9123,13 @@
         <v>53</v>
       </c>
       <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="10" t="s">
         <v>189</v>
       </c>
@@ -9114,10 +9143,13 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="10" t="s">
         <v>189</v>
       </c>
@@ -9127,11 +9159,11 @@
       <c r="C5" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="10" t="s">
         <v>189</v>
       </c>
@@ -9145,10 +9177,13 @@
         <v>60</v>
       </c>
       <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="10" t="s">
         <v>189</v>
       </c>
@@ -9162,10 +9197,13 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="10" t="s">
         <v>189</v>
       </c>
@@ -9175,11 +9213,11 @@
       <c r="C8" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="G8" s="12" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="10" t="s">
         <v>189</v>
       </c>
@@ -9193,10 +9231,13 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="10" t="s">
         <v>189</v>
       </c>
@@ -9210,10 +9251,13 @@
         <v>34</v>
       </c>
       <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" s="10" t="s">
         <v>189</v>
       </c>
@@ -9223,11 +9267,11 @@
       <c r="C11" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="G11" s="12" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" s="10" t="s">
         <v>189</v>
       </c>
@@ -9241,10 +9285,13 @@
         <v>45</v>
       </c>
       <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="10" t="s">
         <v>189</v>
       </c>
@@ -9258,10 +9305,13 @@
         <v>19</v>
       </c>
       <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="10" t="s">
         <v>189</v>
       </c>
@@ -9271,11 +9321,11 @@
       <c r="C14" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="G14" s="12" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="10" t="s">
         <v>189</v>
       </c>
@@ -9289,10 +9339,13 @@
         <v>89</v>
       </c>
       <c r="E15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" s="10" t="s">
         <v>189</v>
       </c>
@@ -9306,10 +9359,13 @@
         <v>82</v>
       </c>
       <c r="E16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="10" t="s">
         <v>189</v>
       </c>
@@ -9323,10 +9379,13 @@
         <v>74</v>
       </c>
       <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" s="10" t="s">
         <v>189</v>
       </c>
@@ -9340,10 +9399,13 @@
         <v>41</v>
       </c>
       <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" s="10" t="s">
         <v>189</v>
       </c>
@@ -9353,11 +9415,11 @@
       <c r="C19" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="G19" s="12" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" s="10" t="s">
         <v>189</v>
       </c>
@@ -9371,10 +9433,13 @@
         <v>27</v>
       </c>
       <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" s="10" t="s">
         <v>189</v>
       </c>
@@ -9384,11 +9449,11 @@
       <c r="C21" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="G21" s="12" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>173</v>
       </c>
@@ -9402,11 +9467,14 @@
         <v>397</v>
       </c>
       <c r="E22" t="s">
+        <v>398</v>
+      </c>
+      <c r="F22" t="s">
         <v>705</v>
       </c>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>173</v>
       </c>
@@ -9420,11 +9488,14 @@
         <v>412</v>
       </c>
       <c r="E23" t="s">
+        <v>413</v>
+      </c>
+      <c r="F23" t="s">
         <v>705</v>
       </c>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>173</v>
       </c>
@@ -9438,11 +9509,14 @@
         <v>405</v>
       </c>
       <c r="E24" t="s">
+        <v>406</v>
+      </c>
+      <c r="F24" t="s">
         <v>705</v>
       </c>
-      <c r="G24" s="12"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>173</v>
       </c>
@@ -9456,11 +9530,14 @@
         <v>78</v>
       </c>
       <c r="E25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" t="s">
         <v>705</v>
       </c>
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25" s="12"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>173</v>
       </c>
@@ -9474,11 +9551,14 @@
         <v>89</v>
       </c>
       <c r="E26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" t="s">
         <v>705</v>
       </c>
-      <c r="G26" s="12"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" s="12"/>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>173</v>
       </c>
@@ -9492,11 +9572,14 @@
         <v>82</v>
       </c>
       <c r="E27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" t="s">
         <v>705</v>
       </c>
-      <c r="G27" s="12"/>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>162</v>
       </c>
@@ -9510,11 +9593,14 @@
         <v>78</v>
       </c>
       <c r="E28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" t="s">
         <v>705</v>
       </c>
-      <c r="G28" s="12"/>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" s="12"/>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>162</v>
       </c>
@@ -9528,12 +9614,15 @@
         <v>160</v>
       </c>
       <c r="E29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F29" t="s">
         <v>705</v>
       </c>
-      <c r="F29" s="12"/>
       <c r="G29" s="12"/>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" s="12"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -9543,12 +9632,12 @@
       <c r="C30" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>777</v>
       </c>
-      <c r="G30" s="12"/>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="12"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>162</v>
       </c>
@@ -9558,12 +9647,12 @@
       <c r="C31" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>777</v>
       </c>
-      <c r="G31" s="12"/>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" s="12"/>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>162</v>
       </c>
@@ -9573,12 +9662,12 @@
       <c r="C32" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>777</v>
       </c>
-      <c r="G32" s="12"/>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="12"/>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>162</v>
       </c>
@@ -9588,12 +9677,12 @@
       <c r="C33" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>777</v>
       </c>
-      <c r="G33" s="12"/>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="12"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>162</v>
       </c>
@@ -9607,11 +9696,14 @@
         <v>89</v>
       </c>
       <c r="E34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" t="s">
         <v>705</v>
       </c>
-      <c r="G34" s="12"/>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" s="12"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>162</v>
       </c>
@@ -9625,11 +9717,14 @@
         <v>82</v>
       </c>
       <c r="E35" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" t="s">
         <v>705</v>
       </c>
-      <c r="G35" s="12"/>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="12"/>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>154</v>
       </c>
@@ -9643,10 +9738,13 @@
         <v>78</v>
       </c>
       <c r="E36" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>154</v>
       </c>
@@ -9660,13 +9758,16 @@
         <v>152</v>
       </c>
       <c r="E37" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37" t="s">
         <v>706</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>154</v>
       </c>
@@ -9678,10 +9779,13 @@
         <v>283</v>
       </c>
       <c r="E38" t="s">
+        <v>284</v>
+      </c>
+      <c r="F38" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>154</v>
       </c>
@@ -9693,10 +9797,13 @@
         <v>280</v>
       </c>
       <c r="E39" t="s">
+        <v>281</v>
+      </c>
+      <c r="F39" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>154</v>
       </c>
@@ -9708,10 +9815,13 @@
         <v>265</v>
       </c>
       <c r="E40" t="s">
+        <v>266</v>
+      </c>
+      <c r="F40" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>154</v>
       </c>
@@ -9723,10 +9833,13 @@
         <v>268</v>
       </c>
       <c r="E41" t="s">
+        <v>269</v>
+      </c>
+      <c r="F41" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -9738,10 +9851,13 @@
         <v>262</v>
       </c>
       <c r="E42" t="s">
+        <v>263</v>
+      </c>
+      <c r="F42" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>154</v>
       </c>
@@ -9753,10 +9869,13 @@
         <v>271</v>
       </c>
       <c r="E43" t="s">
+        <v>272</v>
+      </c>
+      <c r="F43" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>154</v>
       </c>
@@ -9768,10 +9887,13 @@
         <v>277</v>
       </c>
       <c r="E44" t="s">
+        <v>278</v>
+      </c>
+      <c r="F44" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>154</v>
       </c>
@@ -9783,10 +9905,13 @@
         <v>274</v>
       </c>
       <c r="E45" t="s">
+        <v>275</v>
+      </c>
+      <c r="F45" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>154</v>
       </c>
@@ -9796,11 +9921,11 @@
       <c r="C46" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>803</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>154</v>
       </c>
@@ -9810,11 +9935,11 @@
       <c r="C47" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>154</v>
       </c>
@@ -9824,11 +9949,11 @@
       <c r="C48" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>154</v>
       </c>
@@ -9838,11 +9963,11 @@
       <c r="C49" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>154</v>
       </c>
@@ -9856,13 +9981,16 @@
         <v>386</v>
       </c>
       <c r="E50" t="s">
+        <v>389</v>
+      </c>
+      <c r="F50" t="s">
         <v>705</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>154</v>
       </c>
@@ -9872,11 +10000,11 @@
       <c r="C51" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>154</v>
       </c>
@@ -9886,11 +10014,11 @@
       <c r="C52" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>154</v>
       </c>
@@ -9904,10 +10032,13 @@
         <v>89</v>
       </c>
       <c r="E53" t="s">
+        <v>92</v>
+      </c>
+      <c r="F53" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>154</v>
       </c>
@@ -9921,10 +10052,13 @@
         <v>82</v>
       </c>
       <c r="E54" t="s">
+        <v>83</v>
+      </c>
+      <c r="F54" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:8">
       <c r="A55" s="10" t="s">
         <v>146</v>
       </c>
@@ -9938,11 +10072,14 @@
         <v>78</v>
       </c>
       <c r="E55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F55" t="s">
         <v>705</v>
       </c>
-      <c r="G55" s="10"/>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="H55" s="10"/>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="10" t="s">
         <v>146</v>
       </c>
@@ -9952,12 +10089,12 @@
       <c r="C56" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>802</v>
       </c>
-      <c r="G56" s="10"/>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56" s="10"/>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="10" t="s">
         <v>146</v>
       </c>
@@ -9971,14 +10108,17 @@
         <v>501</v>
       </c>
       <c r="E57" t="s">
+        <v>504</v>
+      </c>
+      <c r="F57" t="s">
         <v>705</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>801</v>
       </c>
-      <c r="G57" s="10"/>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="H57" s="10"/>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="10" t="s">
         <v>146</v>
       </c>
@@ -9992,14 +10132,17 @@
         <v>144</v>
       </c>
       <c r="E58" t="s">
+        <v>147</v>
+      </c>
+      <c r="F58" t="s">
         <v>706</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>849</v>
       </c>
-      <c r="G58" s="10"/>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58" s="10"/>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="10" t="s">
         <v>146</v>
       </c>
@@ -10010,11 +10153,14 @@
         <v>212</v>
       </c>
       <c r="E59" t="s">
+        <v>213</v>
+      </c>
+      <c r="F59" t="s">
         <v>705</v>
       </c>
-      <c r="G59" s="10"/>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="H59" s="10"/>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="10" t="s">
         <v>146</v>
       </c>
@@ -10025,11 +10171,14 @@
         <v>168</v>
       </c>
       <c r="E60" t="s">
+        <v>169</v>
+      </c>
+      <c r="F60" t="s">
         <v>705</v>
       </c>
-      <c r="G60" s="10"/>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="H60" s="10"/>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="10" t="s">
         <v>146</v>
       </c>
@@ -10041,11 +10190,14 @@
         <v>157</v>
       </c>
       <c r="E61" t="s">
+        <v>158</v>
+      </c>
+      <c r="F61" t="s">
         <v>705</v>
       </c>
-      <c r="G61" s="10"/>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="H61" s="10"/>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="10" t="s">
         <v>146</v>
       </c>
@@ -10057,11 +10209,14 @@
         <v>149</v>
       </c>
       <c r="E62" t="s">
+        <v>150</v>
+      </c>
+      <c r="F62" t="s">
         <v>705</v>
       </c>
-      <c r="G62" s="10"/>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="H62" s="10"/>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="10" t="s">
         <v>146</v>
       </c>
@@ -10071,12 +10226,12 @@
       <c r="C63" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>777</v>
       </c>
-      <c r="G63" s="10"/>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="H63" s="10"/>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="10" t="s">
         <v>146</v>
       </c>
@@ -10086,12 +10241,12 @@
       <c r="C64" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>777</v>
       </c>
-      <c r="G64" s="10"/>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="H64" s="10"/>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="10" t="s">
         <v>146</v>
       </c>
@@ -10101,12 +10256,12 @@
       <c r="C65" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>777</v>
       </c>
-      <c r="G65" s="10"/>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="H65" s="10"/>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="10" t="s">
         <v>146</v>
       </c>
@@ -10120,14 +10275,17 @@
         <v>386</v>
       </c>
       <c r="E66" t="s">
+        <v>389</v>
+      </c>
+      <c r="F66" t="s">
         <v>705</v>
       </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>800</v>
       </c>
-      <c r="G66" s="10"/>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="H66" s="10"/>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="10" t="s">
         <v>146</v>
       </c>
@@ -10137,12 +10295,12 @@
       <c r="C67" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F67" t="s">
+      <c r="G67" t="s">
         <v>777</v>
       </c>
-      <c r="G67" s="10"/>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="10" t="s">
         <v>146</v>
       </c>
@@ -10156,11 +10314,14 @@
         <v>89</v>
       </c>
       <c r="E68" t="s">
+        <v>92</v>
+      </c>
+      <c r="F68" t="s">
         <v>705</v>
       </c>
-      <c r="G68" s="10"/>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="H68" s="10"/>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="10" t="s">
         <v>146</v>
       </c>
@@ -10174,11 +10335,14 @@
         <v>82</v>
       </c>
       <c r="E69" t="s">
+        <v>83</v>
+      </c>
+      <c r="F69" t="s">
         <v>705</v>
       </c>
-      <c r="G69" s="10"/>
-    </row>
-    <row r="70" spans="1:7">
+      <c r="H69" s="10"/>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="10" t="s">
         <v>132</v>
       </c>
@@ -10192,14 +10356,17 @@
         <v>428</v>
       </c>
       <c r="E70" t="s">
+        <v>429</v>
+      </c>
+      <c r="F70" t="s">
         <v>705</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>850</v>
       </c>
-      <c r="G70" s="10"/>
-    </row>
-    <row r="71" spans="1:7">
+      <c r="H70" s="10"/>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="10" t="s">
         <v>132</v>
       </c>
@@ -10213,11 +10380,14 @@
         <v>485</v>
       </c>
       <c r="E71" t="s">
+        <v>486</v>
+      </c>
+      <c r="F71" t="s">
         <v>705</v>
       </c>
-      <c r="G71" s="10"/>
-    </row>
-    <row r="72" spans="1:7">
+      <c r="H71" s="10"/>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="10" t="s">
         <v>132</v>
       </c>
@@ -10231,11 +10401,14 @@
         <v>473</v>
       </c>
       <c r="E72" t="s">
+        <v>474</v>
+      </c>
+      <c r="F72" t="s">
         <v>705</v>
       </c>
-      <c r="G72" s="10"/>
-    </row>
-    <row r="73" spans="1:7">
+      <c r="H72" s="10"/>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="10" t="s">
         <v>132</v>
       </c>
@@ -10249,11 +10422,14 @@
         <v>481</v>
       </c>
       <c r="E73" t="s">
+        <v>482</v>
+      </c>
+      <c r="F73" t="s">
         <v>705</v>
       </c>
-      <c r="G73" s="10"/>
-    </row>
-    <row r="74" spans="1:7">
+      <c r="H73" s="10"/>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="10" t="s">
         <v>132</v>
       </c>
@@ -10267,11 +10443,14 @@
         <v>477</v>
       </c>
       <c r="E74" t="s">
+        <v>478</v>
+      </c>
+      <c r="F74" t="s">
         <v>705</v>
       </c>
-      <c r="G74" s="10"/>
-    </row>
-    <row r="75" spans="1:7">
+      <c r="H74" s="10"/>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="10" t="s">
         <v>132</v>
       </c>
@@ -10285,14 +10464,17 @@
         <v>432</v>
       </c>
       <c r="E75" t="s">
+        <v>433</v>
+      </c>
+      <c r="F75" t="s">
         <v>705</v>
       </c>
-      <c r="F75" t="s">
+      <c r="G75" t="s">
         <v>850</v>
       </c>
-      <c r="G75" s="10"/>
-    </row>
-    <row r="76" spans="1:7">
+      <c r="H75" s="10"/>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" s="10" t="s">
         <v>132</v>
       </c>
@@ -10306,11 +10488,14 @@
         <v>436</v>
       </c>
       <c r="E76" t="s">
+        <v>437</v>
+      </c>
+      <c r="F76" t="s">
         <v>705</v>
       </c>
-      <c r="G76" s="10"/>
-    </row>
-    <row r="77" spans="1:7">
+      <c r="H76" s="10"/>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" s="10" t="s">
         <v>132</v>
       </c>
@@ -10320,12 +10505,12 @@
       <c r="C77" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F77" t="s">
+      <c r="G77" t="s">
         <v>777</v>
       </c>
-      <c r="G77" s="10"/>
-    </row>
-    <row r="78" spans="1:7">
+      <c r="H77" s="10"/>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" s="10" t="s">
         <v>132</v>
       </c>
@@ -10339,11 +10524,14 @@
         <v>89</v>
       </c>
       <c r="E78" t="s">
+        <v>92</v>
+      </c>
+      <c r="F78" t="s">
         <v>705</v>
       </c>
-      <c r="G78" s="10"/>
-    </row>
-    <row r="79" spans="1:7">
+      <c r="H78" s="10"/>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" s="10" t="s">
         <v>132</v>
       </c>
@@ -10357,11 +10545,14 @@
         <v>82</v>
       </c>
       <c r="E79" t="s">
+        <v>83</v>
+      </c>
+      <c r="F79" t="s">
         <v>705</v>
       </c>
-      <c r="G79" s="10"/>
-    </row>
-    <row r="80" spans="1:7">
+      <c r="H79" s="10"/>
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>123</v>
       </c>
@@ -10375,10 +10566,13 @@
         <v>373</v>
       </c>
       <c r="E80" t="s">
+        <v>374</v>
+      </c>
+      <c r="F80" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>123</v>
       </c>
@@ -10392,13 +10586,16 @@
         <v>369</v>
       </c>
       <c r="E81" t="s">
+        <v>370</v>
+      </c>
+      <c r="F81" t="s">
         <v>705</v>
       </c>
-      <c r="F81" t="s">
+      <c r="G81" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>123</v>
       </c>
@@ -10412,10 +10609,13 @@
         <v>365</v>
       </c>
       <c r="E82" t="s">
+        <v>366</v>
+      </c>
+      <c r="F82" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>123</v>
       </c>
@@ -10429,10 +10629,13 @@
         <v>333</v>
       </c>
       <c r="E83" t="s">
+        <v>334</v>
+      </c>
+      <c r="F83" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>123</v>
       </c>
@@ -10446,10 +10649,13 @@
         <v>337</v>
       </c>
       <c r="E84" t="s">
+        <v>338</v>
+      </c>
+      <c r="F84" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>123</v>
       </c>
@@ -10463,10 +10669,13 @@
         <v>382</v>
       </c>
       <c r="E85" t="s">
+        <v>383</v>
+      </c>
+      <c r="F85" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>123</v>
       </c>
@@ -10480,10 +10689,13 @@
         <v>329</v>
       </c>
       <c r="E86" t="s">
+        <v>330</v>
+      </c>
+      <c r="F86" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>123</v>
       </c>
@@ -10497,10 +10709,13 @@
         <v>377</v>
       </c>
       <c r="E87" t="s">
+        <v>380</v>
+      </c>
+      <c r="F87" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>123</v>
       </c>
@@ -10514,10 +10729,13 @@
         <v>89</v>
       </c>
       <c r="E88" t="s">
+        <v>92</v>
+      </c>
+      <c r="F88" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>123</v>
       </c>
@@ -10531,10 +10749,13 @@
         <v>82</v>
       </c>
       <c r="E89" t="s">
+        <v>83</v>
+      </c>
+      <c r="F89" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>114</v>
       </c>
@@ -10548,10 +10769,13 @@
         <v>78</v>
       </c>
       <c r="E90" t="s">
+        <v>79</v>
+      </c>
+      <c r="F90" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>114</v>
       </c>
@@ -10561,11 +10785,11 @@
       <c r="C91" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F91" t="s">
+      <c r="G91" t="s">
         <v>852</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>114</v>
       </c>
@@ -10575,11 +10799,11 @@
       <c r="C92" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F92" t="s">
+      <c r="G92" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>114</v>
       </c>
@@ -10589,11 +10813,11 @@
       <c r="C93" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>114</v>
       </c>
@@ -10607,13 +10831,16 @@
         <v>112</v>
       </c>
       <c r="E94" t="s">
+        <v>115</v>
+      </c>
+      <c r="F94" t="s">
         <v>706</v>
       </c>
-      <c r="F94" s="1" t="s">
+      <c r="G94" s="1" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>114</v>
       </c>
@@ -10627,11 +10854,14 @@
         <v>259</v>
       </c>
       <c r="E95" t="s">
+        <v>260</v>
+      </c>
+      <c r="F95" t="s">
         <v>705</v>
       </c>
-      <c r="F95" s="1"/>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="G95" s="1"/>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>114</v>
       </c>
@@ -10645,11 +10875,14 @@
         <v>256</v>
       </c>
       <c r="E96" t="s">
+        <v>257</v>
+      </c>
+      <c r="F96" t="s">
         <v>705</v>
       </c>
-      <c r="F96" s="1"/>
-    </row>
-    <row r="97" spans="1:7">
+      <c r="G96" s="1"/>
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -10663,11 +10896,14 @@
         <v>253</v>
       </c>
       <c r="E97" t="s">
+        <v>254</v>
+      </c>
+      <c r="F97" t="s">
         <v>705</v>
       </c>
-      <c r="F97" s="1"/>
-    </row>
-    <row r="98" spans="1:7">
+      <c r="G97" s="1"/>
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>114</v>
       </c>
@@ -10681,11 +10917,14 @@
         <v>250</v>
       </c>
       <c r="E98" t="s">
+        <v>251</v>
+      </c>
+      <c r="F98" t="s">
         <v>705</v>
       </c>
-      <c r="F98" s="1"/>
-    </row>
-    <row r="99" spans="1:7">
+      <c r="G98" s="1"/>
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>114</v>
       </c>
@@ -10699,11 +10938,14 @@
         <v>247</v>
       </c>
       <c r="E99" t="s">
+        <v>248</v>
+      </c>
+      <c r="F99" t="s">
         <v>705</v>
       </c>
-      <c r="F99" s="1"/>
-    </row>
-    <row r="100" spans="1:7">
+      <c r="G99" s="1"/>
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>114</v>
       </c>
@@ -10717,11 +10959,14 @@
         <v>244</v>
       </c>
       <c r="E100" t="s">
+        <v>245</v>
+      </c>
+      <c r="F100" t="s">
         <v>705</v>
       </c>
-      <c r="F100" s="1"/>
-    </row>
-    <row r="101" spans="1:7">
+      <c r="G100" s="1"/>
+    </row>
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
         <v>114</v>
       </c>
@@ -10731,11 +10976,11 @@
       <c r="C101" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F101" t="s">
+      <c r="G101" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>114</v>
       </c>
@@ -10745,11 +10990,11 @@
       <c r="C102" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F102" t="s">
+      <c r="G102" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>114</v>
       </c>
@@ -10763,10 +11008,13 @@
         <v>89</v>
       </c>
       <c r="E103" t="s">
+        <v>92</v>
+      </c>
+      <c r="F103" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
         <v>114</v>
       </c>
@@ -10780,10 +11028,13 @@
         <v>82</v>
       </c>
       <c r="E104" t="s">
+        <v>83</v>
+      </c>
+      <c r="F104" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:8">
       <c r="A105" s="10" t="s">
         <v>106</v>
       </c>
@@ -10797,11 +11048,14 @@
         <v>420</v>
       </c>
       <c r="E105" t="s">
+        <v>421</v>
+      </c>
+      <c r="F105" t="s">
         <v>705</v>
       </c>
-      <c r="G105" s="10"/>
-    </row>
-    <row r="106" spans="1:7">
+      <c r="H105" s="10"/>
+    </row>
+    <row r="106" spans="1:8">
       <c r="A106" s="10" t="s">
         <v>106</v>
       </c>
@@ -10815,11 +11069,14 @@
         <v>424</v>
       </c>
       <c r="E106" t="s">
+        <v>425</v>
+      </c>
+      <c r="F106" t="s">
         <v>705</v>
       </c>
-      <c r="G106" s="10"/>
-    </row>
-    <row r="107" spans="1:7">
+      <c r="H106" s="10"/>
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107" s="10" t="s">
         <v>106</v>
       </c>
@@ -10829,12 +11086,12 @@
       <c r="C107" s="13" t="s">
         <v>714</v>
       </c>
-      <c r="F107" t="s">
+      <c r="G107" t="s">
         <v>777</v>
       </c>
-      <c r="G107" s="10"/>
-    </row>
-    <row r="108" spans="1:7">
+      <c r="H107" s="10"/>
+    </row>
+    <row r="108" spans="1:8">
       <c r="A108" s="10" t="s">
         <v>106</v>
       </c>
@@ -10848,11 +11105,14 @@
         <v>393</v>
       </c>
       <c r="E108" t="s">
+        <v>394</v>
+      </c>
+      <c r="F108" t="s">
         <v>705</v>
       </c>
-      <c r="G108" s="10"/>
-    </row>
-    <row r="109" spans="1:7">
+      <c r="H108" s="10"/>
+    </row>
+    <row r="109" spans="1:8">
       <c r="A109" s="10" t="s">
         <v>106</v>
       </c>
@@ -10865,12 +11125,12 @@
       <c r="D109" s="17" t="s">
         <v>859</v>
       </c>
-      <c r="F109" t="s">
+      <c r="G109" t="s">
         <v>858</v>
       </c>
-      <c r="G109" s="10"/>
-    </row>
-    <row r="110" spans="1:7">
+      <c r="H109" s="10"/>
+    </row>
+    <row r="110" spans="1:8">
       <c r="A110" s="10" t="s">
         <v>106</v>
       </c>
@@ -10884,11 +11144,14 @@
         <v>416</v>
       </c>
       <c r="E110" t="s">
+        <v>417</v>
+      </c>
+      <c r="F110" t="s">
         <v>705</v>
       </c>
-      <c r="G110" s="10"/>
-    </row>
-    <row r="111" spans="1:7">
+      <c r="H110" s="10"/>
+    </row>
+    <row r="111" spans="1:8">
       <c r="A111" s="10" t="s">
         <v>106</v>
       </c>
@@ -10902,11 +11165,14 @@
         <v>408</v>
       </c>
       <c r="E111" t="s">
+        <v>409</v>
+      </c>
+      <c r="F111" t="s">
         <v>705</v>
       </c>
-      <c r="G111" s="10"/>
-    </row>
-    <row r="112" spans="1:7">
+      <c r="H111" s="10"/>
+    </row>
+    <row r="112" spans="1:8">
       <c r="A112" s="10" t="s">
         <v>106</v>
       </c>
@@ -10920,11 +11186,14 @@
         <v>89</v>
       </c>
       <c r="E112" t="s">
+        <v>92</v>
+      </c>
+      <c r="F112" t="s">
         <v>705</v>
       </c>
-      <c r="G112" s="10"/>
-    </row>
-    <row r="113" spans="1:7">
+      <c r="H112" s="10"/>
+    </row>
+    <row r="113" spans="1:8">
       <c r="A113" s="10" t="s">
         <v>758</v>
       </c>
@@ -10938,11 +11207,14 @@
         <v>78</v>
       </c>
       <c r="E113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F113" t="s">
         <v>705</v>
       </c>
-      <c r="G113" s="10"/>
-    </row>
-    <row r="114" spans="1:7">
+      <c r="H113" s="10"/>
+    </row>
+    <row r="114" spans="1:8">
       <c r="A114" s="10" t="s">
         <v>758</v>
       </c>
@@ -10952,12 +11224,12 @@
       <c r="C114" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F114" t="s">
-        <v>861</v>
-      </c>
-      <c r="G114" s="10"/>
-    </row>
-    <row r="115" spans="1:7">
+      <c r="G114" t="s">
+        <v>860</v>
+      </c>
+      <c r="H114" s="10"/>
+    </row>
+    <row r="115" spans="1:8">
       <c r="A115" s="10" t="s">
         <v>758</v>
       </c>
@@ -10967,12 +11239,12 @@
       <c r="C115" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F115" t="s">
-        <v>862</v>
-      </c>
-      <c r="G115" s="10"/>
-    </row>
-    <row r="116" spans="1:7">
+      <c r="G115" t="s">
+        <v>861</v>
+      </c>
+      <c r="H115" s="10"/>
+    </row>
+    <row r="116" spans="1:8">
       <c r="A116" s="10" t="s">
         <v>758</v>
       </c>
@@ -10982,12 +11254,12 @@
       <c r="C116" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F116" t="s">
+      <c r="G116" t="s">
         <v>777</v>
       </c>
-      <c r="G116" s="10"/>
-    </row>
-    <row r="117" spans="1:7">
+      <c r="H116" s="10"/>
+    </row>
+    <row r="117" spans="1:8">
       <c r="A117" s="10" t="s">
         <v>758</v>
       </c>
@@ -10997,141 +11269,141 @@
       <c r="C117" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F117" t="s">
-        <v>874</v>
-      </c>
-      <c r="G117" s="10"/>
-    </row>
-    <row r="118" spans="1:7">
+      <c r="G117" t="s">
+        <v>873</v>
+      </c>
+      <c r="H117" s="10"/>
+    </row>
+    <row r="118" spans="1:8">
       <c r="A118" s="10" t="s">
         <v>758</v>
       </c>
       <c r="B118" s="21" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C118" s="12"/>
       <c r="D118" s="4"/>
-      <c r="F118" t="s">
-        <v>872</v>
-      </c>
-      <c r="G118" s="10"/>
-    </row>
-    <row r="119" spans="1:7">
+      <c r="G118" t="s">
+        <v>871</v>
+      </c>
+      <c r="H118" s="10"/>
+    </row>
+    <row r="119" spans="1:8">
       <c r="A119" s="10" t="s">
         <v>758</v>
       </c>
       <c r="B119" s="21" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C119" s="12"/>
       <c r="D119" s="4"/>
-      <c r="F119" t="s">
-        <v>872</v>
-      </c>
-      <c r="G119" s="10"/>
-    </row>
-    <row r="120" spans="1:7">
+      <c r="G119" t="s">
+        <v>871</v>
+      </c>
+      <c r="H119" s="10"/>
+    </row>
+    <row r="120" spans="1:8">
       <c r="A120" s="10" t="s">
         <v>758</v>
       </c>
       <c r="B120" s="21" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C120" s="12"/>
       <c r="D120" s="4"/>
-      <c r="F120" t="s">
-        <v>872</v>
-      </c>
-      <c r="G120" s="10"/>
-    </row>
-    <row r="121" spans="1:7">
+      <c r="G120" t="s">
+        <v>871</v>
+      </c>
+      <c r="H120" s="10"/>
+    </row>
+    <row r="121" spans="1:8">
       <c r="A121" s="10" t="s">
         <v>758</v>
       </c>
       <c r="B121" s="21" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C121" s="12"/>
       <c r="D121" s="4"/>
-      <c r="E121" s="18"/>
-      <c r="F121" t="s">
-        <v>872</v>
-      </c>
-      <c r="G121" s="10"/>
-    </row>
-    <row r="122" spans="1:7">
+      <c r="F121" s="18"/>
+      <c r="G121" t="s">
+        <v>871</v>
+      </c>
+      <c r="H121" s="10"/>
+    </row>
+    <row r="122" spans="1:8">
       <c r="A122" s="10" t="s">
         <v>758</v>
       </c>
       <c r="B122" s="21" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C122" s="12"/>
       <c r="D122" s="4"/>
-      <c r="E122" s="18"/>
-      <c r="F122" t="s">
-        <v>872</v>
-      </c>
-      <c r="G122" s="10"/>
-    </row>
-    <row r="123" spans="1:7">
+      <c r="F122" s="18"/>
+      <c r="G122" t="s">
+        <v>871</v>
+      </c>
+      <c r="H122" s="10"/>
+    </row>
+    <row r="123" spans="1:8">
       <c r="A123" s="10" t="s">
         <v>758</v>
       </c>
       <c r="B123" s="21" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C123" s="12"/>
       <c r="D123" s="4"/>
-      <c r="F123" t="s">
-        <v>872</v>
-      </c>
-      <c r="G123" s="10"/>
-    </row>
-    <row r="124" spans="1:7">
+      <c r="G123" t="s">
+        <v>871</v>
+      </c>
+      <c r="H123" s="10"/>
+    </row>
+    <row r="124" spans="1:8">
       <c r="A124" s="10" t="s">
         <v>758</v>
       </c>
       <c r="B124" s="21" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C124" s="12"/>
       <c r="D124" s="4"/>
-      <c r="F124" t="s">
-        <v>872</v>
-      </c>
-      <c r="G124" s="10"/>
-    </row>
-    <row r="125" spans="1:7">
+      <c r="G124" t="s">
+        <v>871</v>
+      </c>
+      <c r="H124" s="10"/>
+    </row>
+    <row r="125" spans="1:8">
       <c r="A125" s="10" t="s">
         <v>758</v>
       </c>
       <c r="B125" s="21" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C125" s="12"/>
       <c r="D125" s="4"/>
-      <c r="F125" t="s">
-        <v>872</v>
-      </c>
-      <c r="G125" s="10"/>
-    </row>
-    <row r="126" spans="1:7">
+      <c r="G125" t="s">
+        <v>871</v>
+      </c>
+      <c r="H125" s="10"/>
+    </row>
+    <row r="126" spans="1:8">
       <c r="A126" s="10" t="s">
         <v>758</v>
       </c>
       <c r="B126" s="21" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C126" s="12"/>
       <c r="D126" s="20"/>
-      <c r="E126" s="18"/>
-      <c r="F126" t="s">
-        <v>872</v>
-      </c>
-      <c r="G126" s="10"/>
-    </row>
-    <row r="127" spans="1:7">
+      <c r="F126" s="18"/>
+      <c r="G126" t="s">
+        <v>871</v>
+      </c>
+      <c r="H126" s="10"/>
+    </row>
+    <row r="127" spans="1:8">
       <c r="A127" s="10" t="s">
         <v>758</v>
       </c>
@@ -11144,15 +11416,18 @@
       <c r="D127" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E127" s="14" t="s">
+      <c r="E127" t="s">
+        <v>201</v>
+      </c>
+      <c r="F127" s="14" t="s">
         <v>705</v>
       </c>
-      <c r="F127" s="14" t="s">
-        <v>873</v>
-      </c>
-      <c r="G127" s="10"/>
-    </row>
-    <row r="128" spans="1:7">
+      <c r="G127" s="14" t="s">
+        <v>872</v>
+      </c>
+      <c r="H127" s="10"/>
+    </row>
+    <row r="128" spans="1:8">
       <c r="A128" s="10" t="s">
         <v>758</v>
       </c>
@@ -11165,15 +11440,18 @@
       <c r="D128" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E128" s="14" t="s">
+      <c r="E128" t="s">
+        <v>198</v>
+      </c>
+      <c r="F128" s="14" t="s">
         <v>705</v>
       </c>
-      <c r="F128" s="14" t="s">
-        <v>873</v>
-      </c>
-      <c r="G128" s="10"/>
-    </row>
-    <row r="129" spans="1:7">
+      <c r="G128" s="14" t="s">
+        <v>872</v>
+      </c>
+      <c r="H128" s="10"/>
+    </row>
+    <row r="129" spans="1:8">
       <c r="A129" s="10" t="s">
         <v>758</v>
       </c>
@@ -11186,15 +11464,18 @@
       <c r="D129" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E129" s="14" t="s">
+      <c r="E129" t="s">
+        <v>87</v>
+      </c>
+      <c r="F129" s="14" t="s">
         <v>705</v>
       </c>
-      <c r="F129" s="14" t="s">
-        <v>873</v>
-      </c>
-      <c r="G129" s="10"/>
-    </row>
-    <row r="130" spans="1:7">
+      <c r="G129" s="14" t="s">
+        <v>872</v>
+      </c>
+      <c r="H129" s="10"/>
+    </row>
+    <row r="130" spans="1:8">
       <c r="A130" s="10" t="s">
         <v>758</v>
       </c>
@@ -11207,15 +11488,18 @@
       <c r="D130" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E130" s="14" t="s">
+      <c r="E130" t="s">
+        <v>136</v>
+      </c>
+      <c r="F130" s="14" t="s">
         <v>705</v>
       </c>
-      <c r="F130" s="14" t="s">
-        <v>873</v>
-      </c>
-      <c r="G130" s="10"/>
-    </row>
-    <row r="131" spans="1:7">
+      <c r="G130" s="14" t="s">
+        <v>872</v>
+      </c>
+      <c r="H130" s="10"/>
+    </row>
+    <row r="131" spans="1:8">
       <c r="A131" s="10" t="s">
         <v>758</v>
       </c>
@@ -11226,17 +11510,17 @@
         <v>707</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>875</v>
-      </c>
-      <c r="E131" s="14" t="s">
+        <v>874</v>
+      </c>
+      <c r="F131" s="14" t="s">
         <v>705</v>
       </c>
-      <c r="F131" s="14" t="s">
-        <v>873</v>
-      </c>
-      <c r="G131" s="10"/>
-    </row>
-    <row r="132" spans="1:7">
+      <c r="G131" s="14" t="s">
+        <v>872</v>
+      </c>
+      <c r="H131" s="10"/>
+    </row>
+    <row r="132" spans="1:8">
       <c r="A132" s="10" t="s">
         <v>758</v>
       </c>
@@ -11249,15 +11533,18 @@
       <c r="D132" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E132" s="14" t="s">
+      <c r="E132" t="s">
+        <v>102</v>
+      </c>
+      <c r="F132" s="14" t="s">
         <v>705</v>
       </c>
-      <c r="F132" s="14" t="s">
-        <v>873</v>
-      </c>
-      <c r="G132" s="10"/>
-    </row>
-    <row r="133" spans="1:7">
+      <c r="G132" s="14" t="s">
+        <v>872</v>
+      </c>
+      <c r="H132" s="10"/>
+    </row>
+    <row r="133" spans="1:8">
       <c r="A133" s="10" t="s">
         <v>758</v>
       </c>
@@ -11268,17 +11555,17 @@
         <v>714</v>
       </c>
       <c r="D133" s="14" t="s">
-        <v>876</v>
-      </c>
-      <c r="E133" s="14" t="s">
+        <v>875</v>
+      </c>
+      <c r="F133" s="14" t="s">
         <v>705</v>
       </c>
-      <c r="F133" s="14" t="s">
-        <v>880</v>
-      </c>
-      <c r="G133" s="10"/>
-    </row>
-    <row r="134" spans="1:7">
+      <c r="G133" s="14" t="s">
+        <v>879</v>
+      </c>
+      <c r="H133" s="10"/>
+    </row>
+    <row r="134" spans="1:8">
       <c r="A134" s="10" t="s">
         <v>758</v>
       </c>
@@ -11289,17 +11576,17 @@
         <v>714</v>
       </c>
       <c r="D134" s="19" t="s">
-        <v>877</v>
-      </c>
-      <c r="E134" s="14" t="s">
+        <v>876</v>
+      </c>
+      <c r="F134" s="14" t="s">
         <v>705</v>
       </c>
-      <c r="F134" s="14" t="s">
-        <v>880</v>
-      </c>
-      <c r="G134" s="10"/>
-    </row>
-    <row r="135" spans="1:7">
+      <c r="G134" s="14" t="s">
+        <v>879</v>
+      </c>
+      <c r="H134" s="10"/>
+    </row>
+    <row r="135" spans="1:8">
       <c r="A135" s="10" t="s">
         <v>758</v>
       </c>
@@ -11310,17 +11597,17 @@
         <v>714</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>878</v>
-      </c>
-      <c r="E135" s="14" t="s">
+        <v>877</v>
+      </c>
+      <c r="F135" s="14" t="s">
         <v>705</v>
       </c>
-      <c r="F135" s="14" t="s">
-        <v>880</v>
-      </c>
-      <c r="G135" s="10"/>
-    </row>
-    <row r="136" spans="1:7">
+      <c r="G135" s="14" t="s">
+        <v>879</v>
+      </c>
+      <c r="H135" s="10"/>
+    </row>
+    <row r="136" spans="1:8">
       <c r="A136" s="10" t="s">
         <v>758</v>
       </c>
@@ -11330,12 +11617,12 @@
       <c r="C136" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F136" t="s">
-        <v>879</v>
-      </c>
-      <c r="G136" s="10"/>
-    </row>
-    <row r="137" spans="1:7">
+      <c r="G136" t="s">
+        <v>878</v>
+      </c>
+      <c r="H136" s="10"/>
+    </row>
+    <row r="137" spans="1:8">
       <c r="A137" s="10" t="s">
         <v>758</v>
       </c>
@@ -11349,11 +11636,14 @@
         <v>89</v>
       </c>
       <c r="E137" t="s">
+        <v>92</v>
+      </c>
+      <c r="F137" t="s">
         <v>705</v>
       </c>
-      <c r="G137" s="10"/>
-    </row>
-    <row r="138" spans="1:7">
+      <c r="H137" s="10"/>
+    </row>
+    <row r="138" spans="1:8">
       <c r="A138" s="10" t="s">
         <v>758</v>
       </c>
@@ -11367,11 +11657,14 @@
         <v>82</v>
       </c>
       <c r="E138" t="s">
+        <v>83</v>
+      </c>
+      <c r="F138" t="s">
         <v>705</v>
       </c>
-      <c r="G138" s="10"/>
-    </row>
-    <row r="139" spans="1:7">
+      <c r="H138" s="10"/>
+    </row>
+    <row r="139" spans="1:8">
       <c r="A139" s="10" t="s">
         <v>757</v>
       </c>
@@ -11385,11 +11678,14 @@
         <v>345</v>
       </c>
       <c r="E139" t="s">
+        <v>346</v>
+      </c>
+      <c r="F139" t="s">
         <v>705</v>
       </c>
-      <c r="G139" s="10"/>
-    </row>
-    <row r="140" spans="1:7">
+      <c r="H139" s="10"/>
+    </row>
+    <row r="140" spans="1:8">
       <c r="A140" s="10" t="s">
         <v>757</v>
       </c>
@@ -11403,11 +11699,14 @@
         <v>457</v>
       </c>
       <c r="E140" t="s">
+        <v>458</v>
+      </c>
+      <c r="F140" t="s">
         <v>705</v>
       </c>
-      <c r="G140" s="10"/>
-    </row>
-    <row r="141" spans="1:7">
+      <c r="H140" s="10"/>
+    </row>
+    <row r="141" spans="1:8">
       <c r="A141" s="10" t="s">
         <v>757</v>
       </c>
@@ -11421,11 +11720,14 @@
         <v>461</v>
       </c>
       <c r="E141" t="s">
+        <v>462</v>
+      </c>
+      <c r="F141" t="s">
         <v>705</v>
       </c>
-      <c r="G141" s="10"/>
-    </row>
-    <row r="142" spans="1:7">
+      <c r="H141" s="10"/>
+    </row>
+    <row r="142" spans="1:8">
       <c r="A142" s="10" t="s">
         <v>757</v>
       </c>
@@ -11439,11 +11741,14 @@
         <v>465</v>
       </c>
       <c r="E142" t="s">
+        <v>466</v>
+      </c>
+      <c r="F142" t="s">
         <v>705</v>
       </c>
-      <c r="G142" s="10"/>
-    </row>
-    <row r="143" spans="1:7">
+      <c r="H142" s="10"/>
+    </row>
+    <row r="143" spans="1:8">
       <c r="A143" s="10" t="s">
         <v>757</v>
       </c>
@@ -11457,11 +11762,14 @@
         <v>453</v>
       </c>
       <c r="E143" t="s">
+        <v>454</v>
+      </c>
+      <c r="F143" t="s">
         <v>705</v>
       </c>
-      <c r="G143" s="10"/>
-    </row>
-    <row r="144" spans="1:7">
+      <c r="H143" s="10"/>
+    </row>
+    <row r="144" spans="1:8">
       <c r="A144" s="10" t="s">
         <v>757</v>
       </c>
@@ -11475,11 +11783,14 @@
         <v>449</v>
       </c>
       <c r="E144" t="s">
+        <v>450</v>
+      </c>
+      <c r="F144" t="s">
         <v>705</v>
       </c>
-      <c r="G144" s="10"/>
-    </row>
-    <row r="145" spans="1:7">
+      <c r="H144" s="10"/>
+    </row>
+    <row r="145" spans="1:8">
       <c r="A145" s="10" t="s">
         <v>757</v>
       </c>
@@ -11493,11 +11804,14 @@
         <v>445</v>
       </c>
       <c r="E145" t="s">
+        <v>446</v>
+      </c>
+      <c r="F145" t="s">
         <v>705</v>
       </c>
-      <c r="G145" s="10"/>
-    </row>
-    <row r="146" spans="1:7">
+      <c r="H145" s="10"/>
+    </row>
+    <row r="146" spans="1:8">
       <c r="A146" s="10" t="s">
         <v>757</v>
       </c>
@@ -11510,12 +11824,12 @@
       <c r="D146" s="17" t="s">
         <v>859</v>
       </c>
-      <c r="F146" t="s">
-        <v>860</v>
-      </c>
-      <c r="G146" s="10"/>
-    </row>
-    <row r="147" spans="1:7">
+      <c r="G146" t="s">
+        <v>896</v>
+      </c>
+      <c r="H146" s="10"/>
+    </row>
+    <row r="147" spans="1:8">
       <c r="A147" s="10" t="s">
         <v>757</v>
       </c>
@@ -11525,12 +11839,12 @@
       <c r="C147" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="F147" t="s">
+      <c r="G147" t="s">
         <v>777</v>
       </c>
-      <c r="G147" s="10"/>
-    </row>
-    <row r="148" spans="1:7">
+      <c r="H147" s="10"/>
+    </row>
+    <row r="148" spans="1:8">
       <c r="A148" s="10" t="s">
         <v>757</v>
       </c>
@@ -11544,11 +11858,14 @@
         <v>469</v>
       </c>
       <c r="E148" t="s">
+        <v>470</v>
+      </c>
+      <c r="F148" t="s">
         <v>705</v>
       </c>
-      <c r="G148" s="10"/>
-    </row>
-    <row r="149" spans="1:7">
+      <c r="H148" s="10"/>
+    </row>
+    <row r="149" spans="1:8">
       <c r="A149" s="10" t="s">
         <v>757</v>
       </c>
@@ -11558,12 +11875,12 @@
       <c r="C149" s="15" t="s">
         <v>707</v>
       </c>
-      <c r="F149" t="s">
+      <c r="G149" t="s">
         <v>777</v>
       </c>
-      <c r="G149" s="10"/>
-    </row>
-    <row r="150" spans="1:7">
+      <c r="H149" s="10"/>
+    </row>
+    <row r="150" spans="1:8">
       <c r="A150" s="10" t="s">
         <v>757</v>
       </c>
@@ -11577,11 +11894,14 @@
         <v>361</v>
       </c>
       <c r="E150" t="s">
+        <v>362</v>
+      </c>
+      <c r="F150" t="s">
         <v>705</v>
       </c>
-      <c r="G150" s="10"/>
-    </row>
-    <row r="151" spans="1:7">
+      <c r="H150" s="10"/>
+    </row>
+    <row r="151" spans="1:8">
       <c r="A151" s="10" t="s">
         <v>757</v>
       </c>
@@ -11591,12 +11911,12 @@
       <c r="C151" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="F151" t="s">
+      <c r="G151" t="s">
         <v>777</v>
       </c>
-      <c r="G151" s="10"/>
-    </row>
-    <row r="152" spans="1:7">
+      <c r="H151" s="10"/>
+    </row>
+    <row r="152" spans="1:8">
       <c r="A152" s="10" t="s">
         <v>757</v>
       </c>
@@ -11610,11 +11930,14 @@
         <v>89</v>
       </c>
       <c r="E152" t="s">
+        <v>92</v>
+      </c>
+      <c r="F152" t="s">
         <v>705</v>
       </c>
-      <c r="G152" s="10"/>
-    </row>
-    <row r="153" spans="1:7">
+      <c r="H152" s="10"/>
+    </row>
+    <row r="153" spans="1:8">
       <c r="A153" s="10" t="s">
         <v>757</v>
       </c>
@@ -11628,31 +11951,35 @@
         <v>82</v>
       </c>
       <c r="E153" t="s">
+        <v>83</v>
+      </c>
+      <c r="F153" t="s">
         <v>705</v>
       </c>
-      <c r="G153" s="10"/>
-    </row>
-    <row r="156" spans="1:7">
+      <c r="H153" s="10"/>
+    </row>
+    <row r="156" spans="1:8">
       <c r="A156" t="s">
         <v>854</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:8">
       <c r="B157" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:8">
       <c r="B158" s="6" t="s">
         <v>856</v>
       </c>
       <c r="C158" s="6"/>
       <c r="D158" s="6"/>
+      <c r="E158" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="B118:G135">
-    <sortCondition ref="E118:E135"/>
+  <sortState ref="B118:H135">
     <sortCondition ref="F118:F135"/>
+    <sortCondition ref="G118:G135"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>